<commit_message>
Optuna and some work
</commit_message>
<xml_diff>
--- a/_other/WeekPlan.xlsx
+++ b/_other/WeekPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\exchange\RichLaughter2\_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF341A8-84D8-49E5-ADBB-D4235FDE6B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7BC122-A276-496E-B261-DCA62C4A2A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1216,7 +1216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1295,6 +1295,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1308,7 +1314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1368,6 +1374,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1654,7 +1663,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK3" sqref="AK3"/>
+      <selection pane="bottomLeft" activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,7 +2079,7 @@
       <c r="AI2" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>373</v>
       </c>
       <c r="AL2" s="2" t="s">
@@ -2159,7 +2168,7 @@
       <c r="AI3" s="19" t="s">
         <v>360</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>377</v>
       </c>
       <c r="AL3" s="2" t="s">
@@ -2242,7 +2251,7 @@
       <c r="AI4" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="AJ4" s="2" t="s">
+      <c r="AJ4" s="4" t="s">
         <v>363</v>
       </c>
       <c r="AL4" s="2" t="s">
@@ -2313,7 +2322,7 @@
       <c r="AH5" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="AJ5" s="2" t="s">
+      <c r="AJ5" s="21" t="s">
         <v>364</v>
       </c>
       <c r="AL5" s="2" t="s">

</xml_diff>